<commit_message>
actualizado a la version de php con 8.3
</commit_message>
<xml_diff>
--- a/Archivos/QR_ CEREMONIA PRUEBA DEVELOPER.xlsx
+++ b/Archivos/QR_ CEREMONIA PRUEBA DEVELOPER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F58F625-A025-4764-B849-CF16BC6815D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB64062-C6B1-4D2C-90CD-A9E7C4F58EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB96CF93-ABF4-43BD-96C5-DF55E4B53C04}"/>
+    <workbookView xWindow="-28920" yWindow="7065" windowWidth="29040" windowHeight="15840" xr2:uid="{BB96CF93-ABF4-43BD-96C5-DF55E4B53C04}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA ENVÍO MASIVO QR" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="14.25"/>
@@ -587,13 +587,13 @@
     </row>
     <row r="2" spans="1:6" ht="12.95" customHeight="1">
       <c r="A2" s="8">
-        <v>79982585765</v>
+        <v>435435455</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="10">
-        <v>997645</v>
+        <v>997650</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>6</v>
@@ -609,7 +609,7 @@
   <autoFilter ref="A1:F1" xr:uid="{EB5AF3DA-8D29-482C-AC24-D0FFE1C2452A}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{03EC1D41-A498-48E4-8E13-B87C6C7FF03D}"/>
@@ -620,28 +620,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d" xsi:nil="true"/>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BD689CA66C64E54C96FE3BBB0695E00E" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a5c8dd720e4e05b9cb8ae91ab0cdfc0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815" xmlns:ns3="f7d26785-c8e5-475e-a2b4-a7501147c713" xmlns:ns4="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f2d8e53705b45cc5f5f63120abc9e4a" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -918,27 +896,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d" xsi:nil="true"/>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B6372C-0576-4438-8F61-21D1D6028D3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C3A687D-A3A3-48C4-9BF2-8D52B775FC01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D46A0943-54EF-4003-88C6-D3E44A82FEE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -957,4 +937,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C3A687D-A3A3-48C4-9BF2-8D52B775FC01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B6372C-0576-4438-8F61-21D1D6028D3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ya funciona lo de los invitados
</commit_message>
<xml_diff>
--- a/Archivos/QR_ CEREMONIA PRUEBA DEVELOPER.xlsx
+++ b/Archivos/QR_ CEREMONIA PRUEBA DEVELOPER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB64062-C6B1-4D2C-90CD-A9E7C4F58EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A057EC4D-EF79-4587-B728-B8A4388B741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="7065" windowWidth="29040" windowHeight="15840" xr2:uid="{BB96CF93-ABF4-43BD-96C5-DF55E4B53C04}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="14.25"/>
@@ -587,13 +587,13 @@
     </row>
     <row r="2" spans="1:6" ht="12.95" customHeight="1">
       <c r="A2" s="8">
-        <v>435435455</v>
+        <v>664565464</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="10">
-        <v>997650</v>
+        <v>997653</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>6</v>
@@ -620,6 +620,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d" xsi:nil="true"/>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BD689CA66C64E54C96FE3BBB0695E00E" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a5c8dd720e4e05b9cb8ae91ab0cdfc0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815" xmlns:ns3="f7d26785-c8e5-475e-a2b4-a7501147c713" xmlns:ns4="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f2d8e53705b45cc5f5f63120abc9e4a" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -896,29 +918,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B6372C-0576-4438-8F61-21D1D6028D3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d" xsi:nil="true"/>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C3A687D-A3A3-48C4-9BF2-8D52B775FC01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D46A0943-54EF-4003-88C6-D3E44A82FEE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -937,24 +957,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C3A687D-A3A3-48C4-9BF2-8D52B775FC01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B6372C-0576-4438-8F61-21D1D6028D3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c8bc03f8-ceca-46cf-94df-77b6a2bbec6d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="0a9af45c-a0ec-4fe3-ab0b-ac4dccf0a815"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>